<commit_message>
Added stuff to sidebar
</commit_message>
<xml_diff>
--- a/datasets/Worker Remittances Juarez.xlsx
+++ b/datasets/Worker Remittances Juarez.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jematanevar\OneDrive - University of Texas at El Paso\Documents\DataRep 2\New-Data-Rep\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jematanevar\OneDrive - University of Texas at El Paso\Documents\Final Data REP\New-Data-Rep\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B83270DE-86DB-4C5E-A724-B87129679046}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C07224EF-F5CE-4ACD-A7A1-1D6A17085C79}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{B83270DE-86DB-4C5E-A724-B87129679046}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B1E6E43E-F7EC-46DE-973E-6BFA82D335E3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="6">
   <si>
     <t>Banco de México</t>
   </si>
@@ -35,21 +35,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Apr-Jun 2021</t>
-  </si>
-  <si>
-    <t>Jul-Sep 2021</t>
-  </si>
-  <si>
-    <t>Oct-Dec 2021</t>
-  </si>
-  <si>
-    <t>Jan-Mar 2022</t>
-  </si>
-  <si>
-    <t>Apr-Jun 2022</t>
   </si>
   <si>
     <t>Value</t>
@@ -74,7 +59,7 @@
     <numFmt numFmtId="168" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,14 +92,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,7 +115,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -165,9 +142,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -456,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,10 +446,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -486,7 +460,7 @@
         <v>33.718519999999998</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -497,7 +471,7 @@
         <v>39.227823000000001</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -508,7 +482,7 @@
         <v>39.320171999999999</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -519,7 +493,7 @@
         <v>36.575574000000003</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -530,7 +504,7 @@
         <v>36.917152999999999</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -541,7 +515,7 @@
         <v>40.646439000000001</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,7 +526,7 @@
         <v>36.593265000000002</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -563,7 +537,7 @@
         <v>38.263579999999997</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -574,7 +548,7 @@
         <v>39.270256000000003</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -585,7 +559,7 @@
         <v>50.951853</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -596,7 +570,7 @@
         <v>48.904020000000003</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -607,7 +581,7 @@
         <v>45.260959</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,7 +592,7 @@
         <v>46.122515999999997</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -629,7 +603,7 @@
         <v>51.251584999999999</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -641,7 +615,7 @@
         <v>50.594422999999999</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +626,7 @@
         <v>47.660294</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +637,7 @@
         <v>54.441975999999997</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +648,7 @@
         <v>59.485787999999999</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +659,7 @@
         <v>55.926411000000002</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +670,7 @@
         <v>63.780979000000002</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +681,7 @@
         <v>58.766567999999999</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,7 +692,7 @@
         <v>68.959553999999997</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,7 +703,7 @@
         <v>71.676043000000007</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,7 +714,7 @@
         <v>71.164413999999994</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +725,7 @@
         <v>71.829915999999997</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,7 +736,7 @@
         <v>90.254784000000001</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,7 +747,7 @@
         <v>86.179952999999998</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,7 +758,7 @@
         <v>78.299519000000004</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,7 +769,7 @@
         <v>83.554105000000007</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,7 +780,7 @@
         <v>95.834804000000005</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -817,7 +791,7 @@
         <v>118.79091699999999</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -828,7 +802,7 @@
         <v>98.182467000000003</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,62 +813,62 @@
         <v>107.331221</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="12">
+      <c r="A35" s="7">
+        <v>44287</v>
+      </c>
+      <c r="B35" s="11">
         <v>137.97954799999999</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="12">
+      <c r="A36" s="8">
+        <v>44378</v>
+      </c>
+      <c r="B36" s="11">
         <v>147.30662799999999</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="12">
+      <c r="A37" s="9">
+        <v>44470</v>
+      </c>
+      <c r="B37" s="11">
         <v>125.577155</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="12">
+      <c r="A38" s="6">
+        <v>44562</v>
+      </c>
+      <c r="B38" s="11">
         <v>107.125837</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="12">
+      <c r="A39" s="7">
+        <v>44652</v>
+      </c>
+      <c r="B39" s="11">
         <v>131.32201699999999</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>